<commit_message>
Fixed links to called macros and calls with invalid parameters
</commit_message>
<xml_diff>
--- a/test/acceptance/data/MacroCall.xlsx
+++ b/test/acceptance/data/MacroCall.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="394" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="481" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="CallSheet" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="#MacroSheet" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="CallSheetInvalidParameter" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="#MacroSheet" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" name="date1" vbProcedure="false">#ref!!#ref!</definedName>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>call sheet</t>
   </si>
@@ -41,6 +42,12 @@
   </si>
   <si>
     <t>TestCase2</t>
+  </si>
+  <si>
+    <t>wrongParam</t>
+  </si>
+  <si>
+    <t>TestCaseInvalid</t>
   </si>
   <si>
     <t>param cell</t>
@@ -153,8 +160,8 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A4" activeCellId="0" pane="topLeft" sqref="A4"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -186,7 +193,7 @@
         <v>5</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="4">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.35" outlineLevel="0" r="4">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -206,6 +213,57 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="B5" activeCellId="0" pane="topLeft" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.05" outlineLevel="0" r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.05" outlineLevel="0" r="2">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.05" outlineLevel="0" r="3">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -223,7 +281,7 @@
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.05" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
use table styles to identify table cells, refactoring to support reading data via LibreOffice SDK
</commit_message>
<xml_diff>
--- a/test/acceptance/data/MacroCall.xlsx
+++ b/test/acceptance/data/MacroCall.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="481" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="481" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="CallSheet" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
   <definedNames>
     <definedName function="false" hidden="false" name="date1" vbProcedure="false">#ref!!#ref!</definedName>
     <definedName function="false" hidden="false" name="date2" vbProcedure="false">date!#ref!</definedName>
-    <definedName function="false" hidden="false" name="float" vbProcedure="false">#ref!!$a$1</definedName>
+    <definedName function="false" hidden="false" name="float" vbProcedure="false">#ref!!$A$1</definedName>
     <definedName function="false" hidden="false" name="integer" vbProcedure="false">#ref!!#ref!</definedName>
     <definedName function="false" hidden="false" name="param" vbProcedure="false">'#MacroSheet'!$A$1</definedName>
   </definedNames>
@@ -58,9 +58,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt formatCode="GENERAL" numFmtId="164"/>
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -82,73 +82,89 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FFFF"/>
+        <bgColor rgb="FF00FFFF"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
-    <border diagonalDown="false" diagonalUp="false">
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+  <cellStyleXfs count="21">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
-    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
-    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
-    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
-    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
+  <cellStyles count="7">
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Excel Built-in FitTableCell" xfId="20" builtinId="54" customBuiltin="true"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -160,8 +176,8 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -169,7 +185,7 @@
     <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.05" outlineLevel="0" r="1">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -177,7 +193,7 @@
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.5" outlineLevel="0" r="2">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -185,7 +201,7 @@
         <v>3</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="3">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -193,7 +209,7 @@
         <v>5</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.35" outlineLevel="0" r="4">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -204,7 +220,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -219,8 +235,8 @@
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B5" activeCellId="0" pane="topLeft" sqref="B5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -228,7 +244,7 @@
     <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.05" outlineLevel="0" r="1">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -236,7 +252,7 @@
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.05" outlineLevel="0" r="2">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -244,7 +260,7 @@
         <v>6</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.05" outlineLevel="0" r="3">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -255,7 +271,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -270,8 +286,8 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -279,7 +295,7 @@
     <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.05" outlineLevel="0" r="1">
+    <row r="1" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>8</v>
       </c>
@@ -287,7 +303,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>